<commit_message>
Update Color Relacional e Digrama de Classes.xlsx
</commit_message>
<xml_diff>
--- a/docs/Color Relacional e Digrama de Classes.xlsx
+++ b/docs/Color Relacional e Digrama de Classes.xlsx
@@ -5,19 +5,19 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\EBI\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Usuario\Documents\GitHub\Valcode\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{76B7CAF8-038E-449A-850E-80A0E1CD344A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{523BD63C-C3E9-45B9-A226-85BC23170BEA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{BB101925-B9A6-4918-B38A-822E77899DE9}"/>
+    <workbookView xWindow="-25320" yWindow="-1005" windowWidth="25440" windowHeight="15540" activeTab="1" xr2:uid="{BB101925-B9A6-4918-B38A-822E77899DE9}"/>
   </bookViews>
   <sheets>
     <sheet name="Relacional" sheetId="1" r:id="rId1"/>
     <sheet name="DC" sheetId="2" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm.Print_Area" localSheetId="0">Relacional!$C$1:$Q$33</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">Relacional!$A$1:$S$39</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -623,51 +623,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="18" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="18" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="18" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -682,26 +637,11 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -720,9 +660,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1"/>
@@ -749,29 +686,92 @@
     <xf numFmtId="0" fontId="3" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="6" fillId="10" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="18" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="18" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="18" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -3372,855 +3372,856 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C41603E7-0C2F-45FF-BA70-B6942966EFB8}">
   <dimension ref="A1:S40"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScale="115" zoomScaleNormal="115" zoomScaleSheetLayoutView="85" workbookViewId="0">
-      <selection activeCell="U14" sqref="U14"/>
+    <sheetView showGridLines="0" zoomScale="115" zoomScaleNormal="115" zoomScaleSheetLayoutView="85" workbookViewId="0">
+      <selection sqref="A1:S39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B1" s="67" t="s">
+      <c r="B1" s="44" t="s">
         <v>59</v>
       </c>
-      <c r="C1" s="68"/>
-      <c r="D1" s="68"/>
-      <c r="E1" s="68"/>
-      <c r="F1" s="68"/>
-      <c r="G1" s="68"/>
-      <c r="H1" s="68"/>
-      <c r="I1" s="68"/>
-      <c r="J1" s="68"/>
-      <c r="K1" s="68"/>
-      <c r="L1" s="68"/>
-      <c r="M1" s="68"/>
-      <c r="N1" s="68"/>
-      <c r="O1" s="68"/>
-      <c r="P1" s="68"/>
-      <c r="Q1" s="68"/>
-      <c r="R1" s="69"/>
+      <c r="C1" s="45"/>
+      <c r="D1" s="45"/>
+      <c r="E1" s="45"/>
+      <c r="F1" s="45"/>
+      <c r="G1" s="45"/>
+      <c r="H1" s="45"/>
+      <c r="I1" s="45"/>
+      <c r="J1" s="45"/>
+      <c r="K1" s="45"/>
+      <c r="L1" s="45"/>
+      <c r="M1" s="45"/>
+      <c r="N1" s="45"/>
+      <c r="O1" s="45"/>
+      <c r="P1" s="45"/>
+      <c r="Q1" s="45"/>
+      <c r="R1" s="46"/>
     </row>
     <row r="2" spans="1:19" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B2" s="70"/>
-      <c r="C2" s="71"/>
-      <c r="D2" s="71"/>
-      <c r="E2" s="71"/>
-      <c r="F2" s="71"/>
-      <c r="G2" s="71"/>
-      <c r="H2" s="71"/>
-      <c r="I2" s="71"/>
-      <c r="J2" s="71"/>
-      <c r="K2" s="71"/>
-      <c r="L2" s="71"/>
-      <c r="M2" s="71"/>
-      <c r="N2" s="71"/>
-      <c r="O2" s="71"/>
-      <c r="P2" s="71"/>
-      <c r="Q2" s="71"/>
-      <c r="R2" s="72"/>
+      <c r="B2" s="47"/>
+      <c r="C2" s="48"/>
+      <c r="D2" s="48"/>
+      <c r="E2" s="48"/>
+      <c r="F2" s="48"/>
+      <c r="G2" s="48"/>
+      <c r="H2" s="48"/>
+      <c r="I2" s="48"/>
+      <c r="J2" s="48"/>
+      <c r="K2" s="48"/>
+      <c r="L2" s="48"/>
+      <c r="M2" s="48"/>
+      <c r="N2" s="48"/>
+      <c r="O2" s="48"/>
+      <c r="P2" s="48"/>
+      <c r="Q2" s="48"/>
+      <c r="R2" s="49"/>
     </row>
     <row r="3" spans="1:19" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A3" s="47"/>
-      <c r="B3" s="58"/>
-      <c r="C3" s="57"/>
-      <c r="D3" s="57"/>
-      <c r="E3" s="57"/>
-      <c r="F3" s="57"/>
-      <c r="G3" s="57"/>
-      <c r="H3" s="57"/>
-      <c r="I3" s="57"/>
-      <c r="J3" s="57"/>
-      <c r="K3" s="57"/>
-      <c r="L3" s="57"/>
-      <c r="M3" s="57"/>
-      <c r="N3" s="57"/>
-      <c r="O3" s="57"/>
-      <c r="P3" s="57"/>
-      <c r="Q3" s="57"/>
-      <c r="R3" s="59"/>
-      <c r="S3" s="47"/>
+      <c r="A3" s="27"/>
+      <c r="B3" s="37"/>
+      <c r="C3" s="36"/>
+      <c r="D3" s="36"/>
+      <c r="E3" s="36"/>
+      <c r="F3" s="36"/>
+      <c r="G3" s="36"/>
+      <c r="H3" s="36"/>
+      <c r="I3" s="36"/>
+      <c r="J3" s="36"/>
+      <c r="K3" s="36"/>
+      <c r="L3" s="36"/>
+      <c r="M3" s="36"/>
+      <c r="N3" s="36"/>
+      <c r="O3" s="36"/>
+      <c r="P3" s="36"/>
+      <c r="Q3" s="36"/>
+      <c r="R3" s="38"/>
+      <c r="S3" s="27"/>
     </row>
     <row r="4" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A4" s="47"/>
-      <c r="B4" s="58"/>
-      <c r="C4" s="47"/>
-      <c r="D4" s="47"/>
-      <c r="E4" s="47"/>
-      <c r="F4" s="47"/>
-      <c r="G4" s="47"/>
-      <c r="H4" s="47"/>
-      <c r="I4" s="47"/>
-      <c r="J4" s="47"/>
-      <c r="K4" s="47"/>
-      <c r="L4" s="47"/>
-      <c r="M4" s="47"/>
-      <c r="N4" s="47"/>
-      <c r="O4" s="47"/>
-      <c r="P4" s="47"/>
-      <c r="Q4" s="47"/>
-      <c r="R4" s="59"/>
-      <c r="S4" s="47"/>
+      <c r="A4" s="27"/>
+      <c r="B4" s="37"/>
+      <c r="C4" s="27"/>
+      <c r="D4" s="27"/>
+      <c r="E4" s="27"/>
+      <c r="F4" s="27"/>
+      <c r="G4" s="27"/>
+      <c r="H4" s="27"/>
+      <c r="I4" s="27"/>
+      <c r="J4" s="27"/>
+      <c r="K4" s="27"/>
+      <c r="L4" s="27"/>
+      <c r="M4" s="27"/>
+      <c r="N4" s="27"/>
+      <c r="O4" s="27"/>
+      <c r="P4" s="27"/>
+      <c r="Q4" s="27"/>
+      <c r="R4" s="38"/>
+      <c r="S4" s="27"/>
     </row>
     <row r="5" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A5" s="47"/>
-      <c r="B5" s="58"/>
-      <c r="C5" s="47"/>
-      <c r="D5" s="47"/>
-      <c r="E5" s="47"/>
-      <c r="F5" s="47"/>
-      <c r="G5" s="47"/>
-      <c r="H5" s="47"/>
-      <c r="I5" s="47"/>
-      <c r="J5" s="47"/>
-      <c r="K5" s="47"/>
-      <c r="L5" s="47"/>
-      <c r="M5" s="47"/>
-      <c r="N5" s="47"/>
-      <c r="O5" s="47"/>
-      <c r="P5" s="47"/>
-      <c r="Q5" s="47"/>
-      <c r="R5" s="59"/>
-      <c r="S5" s="47"/>
+      <c r="A5" s="27"/>
+      <c r="B5" s="37"/>
+      <c r="C5" s="27"/>
+      <c r="D5" s="27"/>
+      <c r="E5" s="27"/>
+      <c r="F5" s="27"/>
+      <c r="G5" s="27"/>
+      <c r="H5" s="27"/>
+      <c r="I5" s="27"/>
+      <c r="J5" s="27"/>
+      <c r="K5" s="27"/>
+      <c r="L5" s="27"/>
+      <c r="M5" s="27"/>
+      <c r="N5" s="27"/>
+      <c r="O5" s="27"/>
+      <c r="P5" s="27"/>
+      <c r="Q5" s="27"/>
+      <c r="R5" s="38"/>
+      <c r="S5" s="27"/>
     </row>
     <row r="6" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A6" s="47"/>
-      <c r="B6" s="58"/>
-      <c r="C6" s="47"/>
-      <c r="D6" s="47"/>
-      <c r="E6" s="47"/>
-      <c r="F6" s="47"/>
-      <c r="G6" s="47"/>
-      <c r="H6" s="47"/>
-      <c r="I6" s="47"/>
-      <c r="J6" s="47"/>
-      <c r="K6" s="47"/>
-      <c r="L6" s="47"/>
-      <c r="M6" s="47"/>
-      <c r="N6" s="47"/>
-      <c r="O6" s="47"/>
-      <c r="P6" s="47"/>
-      <c r="Q6" s="47"/>
-      <c r="R6" s="59"/>
-      <c r="S6" s="47"/>
+      <c r="A6" s="27"/>
+      <c r="B6" s="37"/>
+      <c r="C6" s="27"/>
+      <c r="D6" s="27"/>
+      <c r="E6" s="27"/>
+      <c r="F6" s="27"/>
+      <c r="G6" s="27"/>
+      <c r="H6" s="27"/>
+      <c r="I6" s="27"/>
+      <c r="J6" s="27"/>
+      <c r="K6" s="27"/>
+      <c r="L6" s="27"/>
+      <c r="M6" s="27"/>
+      <c r="N6" s="27"/>
+      <c r="O6" s="27"/>
+      <c r="P6" s="27"/>
+      <c r="Q6" s="27"/>
+      <c r="R6" s="38"/>
+      <c r="S6" s="27"/>
     </row>
     <row r="7" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A7" s="47"/>
-      <c r="B7" s="58"/>
-      <c r="C7" s="47"/>
-      <c r="D7" s="47"/>
-      <c r="E7" s="47"/>
-      <c r="F7" s="47"/>
-      <c r="G7" s="47"/>
-      <c r="H7" s="47"/>
-      <c r="I7" s="47"/>
-      <c r="J7" s="47"/>
-      <c r="K7" s="47"/>
-      <c r="L7" s="47"/>
-      <c r="M7" s="47"/>
-      <c r="N7" s="47"/>
-      <c r="O7" s="47"/>
-      <c r="P7" s="47"/>
-      <c r="Q7" s="47"/>
-      <c r="R7" s="59"/>
-      <c r="S7" s="47"/>
+      <c r="A7" s="27"/>
+      <c r="B7" s="37"/>
+      <c r="C7" s="27"/>
+      <c r="D7" s="27"/>
+      <c r="E7" s="27"/>
+      <c r="F7" s="27"/>
+      <c r="G7" s="27"/>
+      <c r="H7" s="27"/>
+      <c r="I7" s="27"/>
+      <c r="J7" s="27"/>
+      <c r="K7" s="27"/>
+      <c r="L7" s="27"/>
+      <c r="M7" s="27"/>
+      <c r="N7" s="27"/>
+      <c r="O7" s="27"/>
+      <c r="P7" s="27"/>
+      <c r="Q7" s="27"/>
+      <c r="R7" s="38"/>
+      <c r="S7" s="27"/>
     </row>
     <row r="8" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A8" s="47"/>
-      <c r="B8" s="58"/>
-      <c r="C8" s="47"/>
-      <c r="D8" s="47"/>
-      <c r="E8" s="47"/>
-      <c r="F8" s="47"/>
-      <c r="G8" s="47"/>
-      <c r="H8" s="47"/>
-      <c r="I8" s="47"/>
-      <c r="J8" s="47"/>
-      <c r="K8" s="47"/>
-      <c r="L8" s="47"/>
-      <c r="M8" s="47"/>
-      <c r="N8" s="47"/>
-      <c r="O8" s="47"/>
-      <c r="P8" s="47"/>
-      <c r="Q8" s="47"/>
-      <c r="R8" s="59"/>
-      <c r="S8" s="47"/>
+      <c r="A8" s="27"/>
+      <c r="B8" s="37"/>
+      <c r="C8" s="27"/>
+      <c r="D8" s="27"/>
+      <c r="E8" s="27"/>
+      <c r="F8" s="27"/>
+      <c r="G8" s="27"/>
+      <c r="H8" s="27"/>
+      <c r="I8" s="27"/>
+      <c r="J8" s="27"/>
+      <c r="K8" s="27"/>
+      <c r="L8" s="27"/>
+      <c r="M8" s="27"/>
+      <c r="N8" s="27"/>
+      <c r="O8" s="27"/>
+      <c r="P8" s="27"/>
+      <c r="Q8" s="27"/>
+      <c r="R8" s="38"/>
+      <c r="S8" s="27"/>
     </row>
     <row r="9" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A9" s="47"/>
-      <c r="B9" s="58"/>
-      <c r="C9" s="47"/>
-      <c r="D9" s="47"/>
-      <c r="E9" s="47"/>
-      <c r="F9" s="47"/>
-      <c r="G9" s="47"/>
-      <c r="H9" s="47"/>
-      <c r="I9" s="47"/>
-      <c r="J9" s="47"/>
-      <c r="K9" s="47"/>
-      <c r="L9" s="47"/>
-      <c r="M9" s="47"/>
-      <c r="N9" s="47"/>
-      <c r="O9" s="47"/>
-      <c r="P9" s="47"/>
-      <c r="Q9" s="47"/>
-      <c r="R9" s="59"/>
-      <c r="S9" s="47"/>
+      <c r="A9" s="27"/>
+      <c r="B9" s="37"/>
+      <c r="C9" s="27"/>
+      <c r="D9" s="27"/>
+      <c r="E9" s="27"/>
+      <c r="F9" s="27"/>
+      <c r="G9" s="27"/>
+      <c r="H9" s="27"/>
+      <c r="I9" s="27"/>
+      <c r="J9" s="27"/>
+      <c r="K9" s="27"/>
+      <c r="L9" s="27"/>
+      <c r="M9" s="27"/>
+      <c r="N9" s="27"/>
+      <c r="O9" s="27"/>
+      <c r="P9" s="27"/>
+      <c r="Q9" s="27"/>
+      <c r="R9" s="38"/>
+      <c r="S9" s="27"/>
     </row>
     <row r="10" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A10" s="47"/>
-      <c r="B10" s="58"/>
-      <c r="C10" s="47"/>
-      <c r="D10" s="47"/>
-      <c r="E10" s="47"/>
-      <c r="F10" s="47"/>
-      <c r="G10" s="47"/>
-      <c r="H10" s="47"/>
-      <c r="I10" s="47"/>
-      <c r="J10" s="47"/>
-      <c r="K10" s="47"/>
-      <c r="L10" s="47"/>
-      <c r="M10" s="47"/>
-      <c r="N10" s="47"/>
-      <c r="O10" s="47"/>
-      <c r="P10" s="47"/>
-      <c r="Q10" s="47"/>
-      <c r="R10" s="59"/>
-      <c r="S10" s="47"/>
+      <c r="A10" s="27"/>
+      <c r="B10" s="37"/>
+      <c r="C10" s="27"/>
+      <c r="D10" s="27"/>
+      <c r="E10" s="27"/>
+      <c r="F10" s="27"/>
+      <c r="G10" s="27"/>
+      <c r="H10" s="27"/>
+      <c r="I10" s="27"/>
+      <c r="J10" s="27"/>
+      <c r="K10" s="27"/>
+      <c r="L10" s="27"/>
+      <c r="M10" s="27"/>
+      <c r="N10" s="27"/>
+      <c r="O10" s="27"/>
+      <c r="P10" s="27"/>
+      <c r="Q10" s="27"/>
+      <c r="R10" s="38"/>
+      <c r="S10" s="27"/>
     </row>
     <row r="11" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A11" s="47"/>
-      <c r="B11" s="58"/>
-      <c r="C11" s="47"/>
-      <c r="D11" s="47"/>
-      <c r="E11" s="47"/>
-      <c r="F11" s="47"/>
-      <c r="G11" s="47"/>
-      <c r="H11" s="47"/>
-      <c r="I11" s="47"/>
-      <c r="J11" s="47"/>
-      <c r="K11" s="47"/>
-      <c r="L11" s="47"/>
-      <c r="M11" s="47"/>
-      <c r="N11" s="47"/>
-      <c r="O11" s="47"/>
-      <c r="P11" s="47"/>
-      <c r="Q11" s="47"/>
-      <c r="R11" s="59"/>
-      <c r="S11" s="47"/>
+      <c r="A11" s="27"/>
+      <c r="B11" s="37"/>
+      <c r="C11" s="27"/>
+      <c r="D11" s="27"/>
+      <c r="E11" s="27"/>
+      <c r="F11" s="27"/>
+      <c r="G11" s="27"/>
+      <c r="H11" s="27"/>
+      <c r="I11" s="27"/>
+      <c r="J11" s="27"/>
+      <c r="K11" s="27"/>
+      <c r="L11" s="27"/>
+      <c r="M11" s="27"/>
+      <c r="N11" s="27"/>
+      <c r="O11" s="27"/>
+      <c r="P11" s="27"/>
+      <c r="Q11" s="27"/>
+      <c r="R11" s="38"/>
+      <c r="S11" s="27"/>
     </row>
     <row r="12" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A12" s="47"/>
-      <c r="B12" s="58"/>
-      <c r="C12" s="47"/>
-      <c r="D12" s="47"/>
-      <c r="E12" s="47"/>
-      <c r="F12" s="47"/>
-      <c r="G12" s="47"/>
-      <c r="H12" s="47"/>
-      <c r="I12" s="47"/>
-      <c r="J12" s="47"/>
-      <c r="K12" s="47"/>
-      <c r="L12" s="47"/>
-      <c r="M12" s="47"/>
-      <c r="N12" s="47"/>
-      <c r="O12" s="47"/>
-      <c r="P12" s="47"/>
-      <c r="Q12" s="47"/>
-      <c r="R12" s="59"/>
-      <c r="S12" s="47"/>
+      <c r="A12" s="27"/>
+      <c r="B12" s="37"/>
+      <c r="C12" s="27"/>
+      <c r="D12" s="27"/>
+      <c r="E12" s="27"/>
+      <c r="F12" s="27"/>
+      <c r="G12" s="27"/>
+      <c r="H12" s="27"/>
+      <c r="I12" s="27"/>
+      <c r="J12" s="27"/>
+      <c r="K12" s="27"/>
+      <c r="L12" s="27"/>
+      <c r="M12" s="27"/>
+      <c r="N12" s="27"/>
+      <c r="O12" s="27"/>
+      <c r="P12" s="27"/>
+      <c r="Q12" s="27"/>
+      <c r="R12" s="38"/>
+      <c r="S12" s="27"/>
     </row>
     <row r="13" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A13" s="47"/>
-      <c r="B13" s="58"/>
-      <c r="C13" s="47"/>
-      <c r="D13" s="47"/>
-      <c r="E13" s="47"/>
-      <c r="F13" s="47"/>
-      <c r="G13" s="47"/>
-      <c r="H13" s="47"/>
-      <c r="I13" s="47"/>
-      <c r="J13" s="47"/>
-      <c r="K13" s="47"/>
-      <c r="L13" s="47"/>
-      <c r="M13" s="47"/>
-      <c r="N13" s="47"/>
-      <c r="O13" s="47"/>
-      <c r="P13" s="47"/>
-      <c r="Q13" s="47"/>
-      <c r="R13" s="59"/>
-      <c r="S13" s="47"/>
+      <c r="A13" s="27"/>
+      <c r="B13" s="37"/>
+      <c r="C13" s="27"/>
+      <c r="D13" s="27"/>
+      <c r="E13" s="27"/>
+      <c r="F13" s="27"/>
+      <c r="G13" s="27"/>
+      <c r="H13" s="27"/>
+      <c r="I13" s="27"/>
+      <c r="J13" s="27"/>
+      <c r="K13" s="27"/>
+      <c r="L13" s="27"/>
+      <c r="M13" s="27"/>
+      <c r="N13" s="27"/>
+      <c r="O13" s="27"/>
+      <c r="P13" s="27"/>
+      <c r="Q13" s="27"/>
+      <c r="R13" s="38"/>
+      <c r="S13" s="27"/>
     </row>
     <row r="14" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A14" s="47"/>
-      <c r="B14" s="58"/>
-      <c r="C14" s="47"/>
-      <c r="D14" s="47"/>
-      <c r="E14" s="47"/>
-      <c r="F14" s="47"/>
-      <c r="G14" s="47"/>
-      <c r="H14" s="47"/>
-      <c r="I14" s="47"/>
-      <c r="J14" s="47"/>
-      <c r="K14" s="47"/>
-      <c r="L14" s="47"/>
-      <c r="M14" s="47"/>
-      <c r="N14" s="47"/>
-      <c r="O14" s="47"/>
-      <c r="P14" s="47"/>
-      <c r="Q14" s="47"/>
-      <c r="R14" s="59"/>
-      <c r="S14" s="47"/>
+      <c r="A14" s="27"/>
+      <c r="B14" s="37"/>
+      <c r="C14" s="27"/>
+      <c r="D14" s="27"/>
+      <c r="E14" s="27"/>
+      <c r="F14" s="27"/>
+      <c r="G14" s="27"/>
+      <c r="H14" s="27"/>
+      <c r="I14" s="27"/>
+      <c r="J14" s="27"/>
+      <c r="K14" s="27"/>
+      <c r="L14" s="27"/>
+      <c r="M14" s="27"/>
+      <c r="N14" s="27"/>
+      <c r="O14" s="27"/>
+      <c r="P14" s="27"/>
+      <c r="Q14" s="27"/>
+      <c r="R14" s="38"/>
+      <c r="S14" s="27"/>
     </row>
     <row r="15" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A15" s="47"/>
-      <c r="B15" s="58"/>
-      <c r="C15" s="47"/>
-      <c r="D15" s="47"/>
-      <c r="E15" s="47"/>
-      <c r="F15" s="47"/>
-      <c r="G15" s="47"/>
-      <c r="H15" s="47"/>
-      <c r="I15" s="47"/>
-      <c r="J15" s="47"/>
-      <c r="K15" s="47"/>
-      <c r="L15" s="47"/>
-      <c r="M15" s="47"/>
-      <c r="N15" s="47"/>
-      <c r="O15" s="47"/>
-      <c r="P15" s="47"/>
-      <c r="Q15" s="47"/>
-      <c r="R15" s="59"/>
-      <c r="S15" s="47"/>
+      <c r="A15" s="27"/>
+      <c r="B15" s="37"/>
+      <c r="C15" s="27"/>
+      <c r="D15" s="27"/>
+      <c r="E15" s="27"/>
+      <c r="F15" s="27"/>
+      <c r="G15" s="27"/>
+      <c r="H15" s="27"/>
+      <c r="I15" s="27"/>
+      <c r="J15" s="27"/>
+      <c r="K15" s="27"/>
+      <c r="L15" s="27"/>
+      <c r="M15" s="27"/>
+      <c r="N15" s="27"/>
+      <c r="O15" s="27"/>
+      <c r="P15" s="27"/>
+      <c r="Q15" s="27"/>
+      <c r="R15" s="38"/>
+      <c r="S15" s="27"/>
     </row>
     <row r="16" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A16" s="47"/>
-      <c r="B16" s="58"/>
-      <c r="C16" s="47"/>
-      <c r="D16" s="47"/>
-      <c r="E16" s="47"/>
-      <c r="F16" s="47"/>
-      <c r="G16" s="47"/>
-      <c r="H16" s="47"/>
-      <c r="I16" s="47"/>
-      <c r="J16" s="47"/>
-      <c r="K16" s="47"/>
-      <c r="L16" s="47"/>
-      <c r="M16" s="47"/>
-      <c r="N16" s="47"/>
-      <c r="O16" s="47"/>
-      <c r="P16" s="47"/>
-      <c r="Q16" s="47"/>
-      <c r="R16" s="59"/>
-      <c r="S16" s="47"/>
+      <c r="A16" s="27"/>
+      <c r="B16" s="37"/>
+      <c r="C16" s="27"/>
+      <c r="D16" s="27"/>
+      <c r="E16" s="27"/>
+      <c r="F16" s="27"/>
+      <c r="G16" s="27"/>
+      <c r="H16" s="27"/>
+      <c r="I16" s="27"/>
+      <c r="J16" s="27"/>
+      <c r="K16" s="27"/>
+      <c r="L16" s="27"/>
+      <c r="M16" s="27"/>
+      <c r="N16" s="27"/>
+      <c r="O16" s="27"/>
+      <c r="P16" s="27"/>
+      <c r="Q16" s="27"/>
+      <c r="R16" s="38"/>
+      <c r="S16" s="27"/>
     </row>
     <row r="17" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A17" s="47"/>
-      <c r="B17" s="58"/>
-      <c r="C17" s="47"/>
-      <c r="D17" s="47"/>
-      <c r="E17" s="47"/>
-      <c r="F17" s="47"/>
-      <c r="G17" s="47"/>
-      <c r="H17" s="47"/>
-      <c r="I17" s="47"/>
-      <c r="J17" s="47"/>
-      <c r="K17" s="47"/>
-      <c r="L17" s="47"/>
-      <c r="M17" s="47"/>
-      <c r="N17" s="47"/>
-      <c r="O17" s="47"/>
-      <c r="P17" s="47"/>
-      <c r="Q17" s="47"/>
-      <c r="R17" s="59"/>
-      <c r="S17" s="47"/>
+      <c r="A17" s="27"/>
+      <c r="B17" s="37"/>
+      <c r="C17" s="27"/>
+      <c r="D17" s="27"/>
+      <c r="E17" s="27"/>
+      <c r="F17" s="27"/>
+      <c r="G17" s="27"/>
+      <c r="H17" s="27"/>
+      <c r="I17" s="27"/>
+      <c r="J17" s="27"/>
+      <c r="K17" s="27"/>
+      <c r="L17" s="27"/>
+      <c r="M17" s="27"/>
+      <c r="N17" s="27"/>
+      <c r="O17" s="27"/>
+      <c r="P17" s="27"/>
+      <c r="Q17" s="27"/>
+      <c r="R17" s="38"/>
+      <c r="S17" s="27"/>
     </row>
     <row r="18" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A18" s="47"/>
-      <c r="B18" s="58"/>
-      <c r="C18" s="47"/>
-      <c r="D18" s="47"/>
-      <c r="E18" s="47"/>
-      <c r="F18" s="47"/>
-      <c r="G18" s="47"/>
-      <c r="H18" s="47"/>
-      <c r="I18" s="47"/>
-      <c r="J18" s="47"/>
-      <c r="K18" s="47"/>
-      <c r="L18" s="47"/>
-      <c r="M18" s="47"/>
-      <c r="N18" s="47"/>
-      <c r="O18" s="47"/>
-      <c r="P18" s="47"/>
-      <c r="Q18" s="47"/>
-      <c r="R18" s="59"/>
-      <c r="S18" s="47"/>
+      <c r="A18" s="27"/>
+      <c r="B18" s="37"/>
+      <c r="C18" s="27"/>
+      <c r="D18" s="27"/>
+      <c r="E18" s="27"/>
+      <c r="F18" s="27"/>
+      <c r="G18" s="27"/>
+      <c r="H18" s="27"/>
+      <c r="I18" s="27"/>
+      <c r="J18" s="27"/>
+      <c r="K18" s="27"/>
+      <c r="L18" s="27"/>
+      <c r="M18" s="27"/>
+      <c r="N18" s="27"/>
+      <c r="O18" s="27"/>
+      <c r="P18" s="27"/>
+      <c r="Q18" s="27"/>
+      <c r="R18" s="38"/>
+      <c r="S18" s="27"/>
     </row>
     <row r="19" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A19" s="47"/>
-      <c r="B19" s="58"/>
-      <c r="C19" s="47"/>
-      <c r="D19" s="47"/>
-      <c r="E19" s="47"/>
-      <c r="F19" s="47"/>
-      <c r="G19" s="47"/>
-      <c r="H19" s="47"/>
-      <c r="I19" s="47"/>
-      <c r="J19" s="47"/>
-      <c r="K19" s="47"/>
-      <c r="L19" s="47"/>
-      <c r="M19" s="47"/>
-      <c r="N19" s="47"/>
-      <c r="O19" s="47"/>
-      <c r="P19" s="47"/>
-      <c r="Q19" s="47"/>
-      <c r="R19" s="59"/>
-      <c r="S19" s="47"/>
+      <c r="A19" s="27"/>
+      <c r="B19" s="37"/>
+      <c r="C19" s="27"/>
+      <c r="D19" s="27"/>
+      <c r="E19" s="27"/>
+      <c r="F19" s="27"/>
+      <c r="G19" s="27"/>
+      <c r="H19" s="27"/>
+      <c r="I19" s="27"/>
+      <c r="J19" s="27"/>
+      <c r="K19" s="27"/>
+      <c r="L19" s="27"/>
+      <c r="M19" s="27"/>
+      <c r="N19" s="27"/>
+      <c r="O19" s="27"/>
+      <c r="P19" s="27"/>
+      <c r="Q19" s="27"/>
+      <c r="R19" s="38"/>
+      <c r="S19" s="27"/>
     </row>
     <row r="20" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A20" s="47"/>
-      <c r="B20" s="58"/>
-      <c r="C20" s="47"/>
-      <c r="D20" s="47"/>
-      <c r="E20" s="47"/>
-      <c r="F20" s="47"/>
-      <c r="G20" s="47"/>
-      <c r="H20" s="47"/>
-      <c r="I20" s="47"/>
-      <c r="J20" s="47"/>
-      <c r="K20" s="47"/>
-      <c r="L20" s="47"/>
-      <c r="M20" s="47"/>
-      <c r="N20" s="47"/>
-      <c r="O20" s="47"/>
-      <c r="P20" s="47"/>
-      <c r="Q20" s="47"/>
-      <c r="R20" s="59"/>
-      <c r="S20" s="47"/>
+      <c r="A20" s="27"/>
+      <c r="B20" s="37"/>
+      <c r="C20" s="27"/>
+      <c r="D20" s="27"/>
+      <c r="E20" s="27"/>
+      <c r="F20" s="27"/>
+      <c r="G20" s="27"/>
+      <c r="H20" s="27"/>
+      <c r="I20" s="27"/>
+      <c r="J20" s="27"/>
+      <c r="K20" s="27"/>
+      <c r="L20" s="27"/>
+      <c r="M20" s="27"/>
+      <c r="N20" s="27"/>
+      <c r="O20" s="27"/>
+      <c r="P20" s="27"/>
+      <c r="Q20" s="27"/>
+      <c r="R20" s="38"/>
+      <c r="S20" s="27"/>
     </row>
     <row r="21" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A21" s="47"/>
-      <c r="B21" s="58"/>
-      <c r="C21" s="47"/>
-      <c r="D21" s="47"/>
-      <c r="E21" s="47"/>
-      <c r="F21" s="47"/>
-      <c r="G21" s="47"/>
-      <c r="H21" s="47"/>
-      <c r="I21" s="47"/>
-      <c r="J21" s="47"/>
-      <c r="K21" s="47"/>
-      <c r="L21" s="47"/>
-      <c r="M21" s="47"/>
-      <c r="N21" s="47"/>
-      <c r="O21" s="47"/>
-      <c r="P21" s="47"/>
-      <c r="Q21" s="47"/>
-      <c r="R21" s="59"/>
-      <c r="S21" s="47"/>
+      <c r="A21" s="27"/>
+      <c r="B21" s="37"/>
+      <c r="C21" s="27"/>
+      <c r="D21" s="27"/>
+      <c r="E21" s="27"/>
+      <c r="F21" s="27"/>
+      <c r="G21" s="27"/>
+      <c r="H21" s="27"/>
+      <c r="I21" s="27"/>
+      <c r="J21" s="27"/>
+      <c r="K21" s="27"/>
+      <c r="L21" s="27"/>
+      <c r="M21" s="27"/>
+      <c r="N21" s="27"/>
+      <c r="O21" s="27"/>
+      <c r="P21" s="27"/>
+      <c r="Q21" s="27"/>
+      <c r="R21" s="38"/>
+      <c r="S21" s="27"/>
     </row>
     <row r="22" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A22" s="47"/>
-      <c r="B22" s="58"/>
-      <c r="C22" s="47"/>
-      <c r="D22" s="47"/>
-      <c r="E22" s="47"/>
-      <c r="F22" s="47"/>
-      <c r="G22" s="47"/>
-      <c r="H22" s="47"/>
-      <c r="I22" s="47"/>
-      <c r="J22" s="47"/>
-      <c r="K22" s="47"/>
-      <c r="L22" s="47"/>
-      <c r="M22" s="47"/>
-      <c r="N22" s="47"/>
-      <c r="O22" s="47"/>
-      <c r="P22" s="47"/>
-      <c r="Q22" s="47"/>
-      <c r="R22" s="59"/>
-      <c r="S22" s="47"/>
+      <c r="A22" s="27"/>
+      <c r="B22" s="37"/>
+      <c r="C22" s="27"/>
+      <c r="D22" s="27"/>
+      <c r="E22" s="27"/>
+      <c r="F22" s="27"/>
+      <c r="G22" s="27"/>
+      <c r="H22" s="27"/>
+      <c r="I22" s="27"/>
+      <c r="J22" s="27"/>
+      <c r="K22" s="27"/>
+      <c r="L22" s="27"/>
+      <c r="M22" s="27"/>
+      <c r="N22" s="27"/>
+      <c r="O22" s="27"/>
+      <c r="P22" s="27"/>
+      <c r="Q22" s="27"/>
+      <c r="R22" s="38"/>
+      <c r="S22" s="27"/>
     </row>
     <row r="23" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A23" s="47"/>
-      <c r="B23" s="58"/>
-      <c r="C23" s="47"/>
-      <c r="D23" s="47"/>
-      <c r="E23" s="47"/>
-      <c r="F23" s="47"/>
-      <c r="G23" s="47"/>
-      <c r="H23" s="47"/>
-      <c r="I23" s="47"/>
-      <c r="J23" s="47"/>
-      <c r="K23" s="47"/>
-      <c r="L23" s="47"/>
-      <c r="M23" s="47"/>
-      <c r="N23" s="47"/>
-      <c r="O23" s="47"/>
-      <c r="P23" s="47"/>
-      <c r="Q23" s="47"/>
-      <c r="R23" s="59"/>
-      <c r="S23" s="47"/>
+      <c r="A23" s="27"/>
+      <c r="B23" s="37"/>
+      <c r="C23" s="27"/>
+      <c r="D23" s="27"/>
+      <c r="E23" s="27"/>
+      <c r="F23" s="27"/>
+      <c r="G23" s="27"/>
+      <c r="H23" s="27"/>
+      <c r="I23" s="27"/>
+      <c r="J23" s="27"/>
+      <c r="K23" s="27"/>
+      <c r="L23" s="27"/>
+      <c r="M23" s="27"/>
+      <c r="N23" s="27"/>
+      <c r="O23" s="27"/>
+      <c r="P23" s="27"/>
+      <c r="Q23" s="27"/>
+      <c r="R23" s="38"/>
+      <c r="S23" s="27"/>
     </row>
     <row r="24" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A24" s="47"/>
-      <c r="B24" s="58"/>
-      <c r="C24" s="47"/>
-      <c r="D24" s="47"/>
-      <c r="E24" s="47"/>
-      <c r="F24" s="47"/>
-      <c r="G24" s="47"/>
-      <c r="H24" s="47"/>
-      <c r="I24" s="47"/>
-      <c r="J24" s="47"/>
-      <c r="K24" s="47"/>
-      <c r="L24" s="47"/>
-      <c r="M24" s="47"/>
-      <c r="N24" s="47"/>
-      <c r="O24" s="47"/>
-      <c r="P24" s="47"/>
-      <c r="Q24" s="47"/>
-      <c r="R24" s="59"/>
-      <c r="S24" s="47"/>
+      <c r="A24" s="27"/>
+      <c r="B24" s="37"/>
+      <c r="C24" s="27"/>
+      <c r="D24" s="27"/>
+      <c r="E24" s="27"/>
+      <c r="F24" s="27"/>
+      <c r="G24" s="27"/>
+      <c r="H24" s="27"/>
+      <c r="I24" s="27"/>
+      <c r="J24" s="27"/>
+      <c r="K24" s="27"/>
+      <c r="L24" s="27"/>
+      <c r="M24" s="27"/>
+      <c r="N24" s="27"/>
+      <c r="O24" s="27"/>
+      <c r="P24" s="27"/>
+      <c r="Q24" s="27"/>
+      <c r="R24" s="38"/>
+      <c r="S24" s="27"/>
     </row>
     <row r="25" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A25" s="47"/>
-      <c r="B25" s="58"/>
-      <c r="C25" s="47"/>
-      <c r="D25" s="47"/>
-      <c r="E25" s="47"/>
-      <c r="F25" s="47"/>
-      <c r="G25" s="47"/>
-      <c r="H25" s="47"/>
-      <c r="I25" s="47"/>
-      <c r="J25" s="47"/>
-      <c r="K25" s="47"/>
-      <c r="L25" s="47"/>
-      <c r="M25" s="47"/>
-      <c r="N25" s="47"/>
-      <c r="O25" s="47"/>
-      <c r="P25" s="47"/>
-      <c r="Q25" s="47"/>
-      <c r="R25" s="59"/>
-      <c r="S25" s="47"/>
+      <c r="A25" s="27"/>
+      <c r="B25" s="37"/>
+      <c r="C25" s="27"/>
+      <c r="D25" s="27"/>
+      <c r="E25" s="27"/>
+      <c r="F25" s="27"/>
+      <c r="G25" s="27"/>
+      <c r="H25" s="27"/>
+      <c r="I25" s="27"/>
+      <c r="J25" s="27"/>
+      <c r="K25" s="27"/>
+      <c r="L25" s="27"/>
+      <c r="M25" s="27"/>
+      <c r="N25" s="27"/>
+      <c r="O25" s="27"/>
+      <c r="P25" s="27"/>
+      <c r="Q25" s="27"/>
+      <c r="R25" s="38"/>
+      <c r="S25" s="27"/>
     </row>
     <row r="26" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A26" s="47"/>
-      <c r="B26" s="58"/>
-      <c r="C26" s="47"/>
-      <c r="D26" s="47"/>
-      <c r="E26" s="47"/>
-      <c r="F26" s="47"/>
-      <c r="G26" s="47"/>
-      <c r="H26" s="47"/>
-      <c r="I26" s="47"/>
-      <c r="J26" s="47"/>
-      <c r="K26" s="47"/>
-      <c r="L26" s="47"/>
-      <c r="M26" s="47"/>
-      <c r="N26" s="47"/>
-      <c r="O26" s="47"/>
-      <c r="P26" s="47"/>
-      <c r="Q26" s="47"/>
-      <c r="R26" s="59"/>
-      <c r="S26" s="47"/>
+      <c r="A26" s="27"/>
+      <c r="B26" s="37"/>
+      <c r="C26" s="27"/>
+      <c r="D26" s="27"/>
+      <c r="E26" s="27"/>
+      <c r="F26" s="27"/>
+      <c r="G26" s="27"/>
+      <c r="H26" s="27"/>
+      <c r="I26" s="27"/>
+      <c r="J26" s="27"/>
+      <c r="K26" s="27"/>
+      <c r="L26" s="27"/>
+      <c r="M26" s="27"/>
+      <c r="N26" s="27"/>
+      <c r="O26" s="27"/>
+      <c r="P26" s="27"/>
+      <c r="Q26" s="27"/>
+      <c r="R26" s="38"/>
+      <c r="S26" s="27"/>
     </row>
     <row r="27" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A27" s="47"/>
-      <c r="B27" s="58"/>
-      <c r="C27" s="47"/>
-      <c r="D27" s="47"/>
-      <c r="E27" s="47"/>
-      <c r="F27" s="47"/>
-      <c r="G27" s="47"/>
-      <c r="H27" s="47"/>
-      <c r="I27" s="47"/>
-      <c r="J27" s="47"/>
-      <c r="K27" s="47"/>
-      <c r="L27" s="47"/>
-      <c r="M27" s="47"/>
-      <c r="N27" s="47"/>
-      <c r="O27" s="47"/>
-      <c r="P27" s="47"/>
-      <c r="Q27" s="47"/>
-      <c r="R27" s="59"/>
-      <c r="S27" s="47"/>
+      <c r="A27" s="27"/>
+      <c r="B27" s="37"/>
+      <c r="C27" s="27"/>
+      <c r="D27" s="27"/>
+      <c r="E27" s="27"/>
+      <c r="F27" s="27"/>
+      <c r="G27" s="27"/>
+      <c r="H27" s="27"/>
+      <c r="I27" s="27"/>
+      <c r="J27" s="27"/>
+      <c r="K27" s="27"/>
+      <c r="L27" s="27"/>
+      <c r="M27" s="27"/>
+      <c r="N27" s="27"/>
+      <c r="O27" s="27"/>
+      <c r="P27" s="27"/>
+      <c r="Q27" s="27"/>
+      <c r="R27" s="38"/>
+      <c r="S27" s="27"/>
     </row>
     <row r="28" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A28" s="47"/>
-      <c r="B28" s="58"/>
-      <c r="C28" s="47"/>
-      <c r="D28" s="47"/>
-      <c r="E28" s="47"/>
-      <c r="F28" s="47"/>
-      <c r="G28" s="47"/>
-      <c r="H28" s="47"/>
-      <c r="I28" s="47"/>
-      <c r="J28" s="47"/>
-      <c r="K28" s="47"/>
-      <c r="L28" s="47"/>
-      <c r="M28" s="47"/>
-      <c r="N28" s="47"/>
-      <c r="O28" s="47"/>
-      <c r="P28" s="47"/>
-      <c r="Q28" s="47"/>
-      <c r="R28" s="59"/>
-      <c r="S28" s="47"/>
+      <c r="A28" s="27"/>
+      <c r="B28" s="37"/>
+      <c r="C28" s="27"/>
+      <c r="D28" s="27"/>
+      <c r="E28" s="27"/>
+      <c r="F28" s="27"/>
+      <c r="G28" s="27"/>
+      <c r="H28" s="27"/>
+      <c r="I28" s="27"/>
+      <c r="J28" s="27"/>
+      <c r="K28" s="27"/>
+      <c r="L28" s="27"/>
+      <c r="M28" s="27"/>
+      <c r="N28" s="27"/>
+      <c r="O28" s="27"/>
+      <c r="P28" s="27"/>
+      <c r="Q28" s="27"/>
+      <c r="R28" s="38"/>
+      <c r="S28" s="27"/>
     </row>
     <row r="29" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A29" s="47"/>
-      <c r="B29" s="58"/>
-      <c r="C29" s="47"/>
-      <c r="D29" s="47"/>
-      <c r="E29" s="47"/>
-      <c r="F29" s="47"/>
-      <c r="G29" s="47"/>
-      <c r="H29" s="47"/>
-      <c r="I29" s="47"/>
-      <c r="J29" s="47"/>
-      <c r="K29" s="47"/>
-      <c r="L29" s="47"/>
-      <c r="M29" s="47"/>
-      <c r="N29" s="47"/>
-      <c r="O29" s="47"/>
-      <c r="P29" s="47"/>
-      <c r="Q29" s="47"/>
-      <c r="R29" s="59"/>
-      <c r="S29" s="47"/>
+      <c r="A29" s="27"/>
+      <c r="B29" s="37"/>
+      <c r="C29" s="27"/>
+      <c r="D29" s="27"/>
+      <c r="E29" s="27"/>
+      <c r="F29" s="27"/>
+      <c r="G29" s="27"/>
+      <c r="H29" s="27"/>
+      <c r="I29" s="27"/>
+      <c r="J29" s="27"/>
+      <c r="K29" s="27"/>
+      <c r="L29" s="27"/>
+      <c r="M29" s="27"/>
+      <c r="N29" s="27"/>
+      <c r="O29" s="27"/>
+      <c r="P29" s="27"/>
+      <c r="Q29" s="27"/>
+      <c r="R29" s="38"/>
+      <c r="S29" s="27"/>
     </row>
     <row r="30" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A30" s="47"/>
-      <c r="B30" s="58"/>
-      <c r="C30" s="47"/>
-      <c r="D30" s="47"/>
-      <c r="E30" s="47"/>
-      <c r="F30" s="47"/>
-      <c r="G30" s="47"/>
-      <c r="H30" s="47"/>
-      <c r="I30" s="47"/>
-      <c r="J30" s="47"/>
-      <c r="K30" s="47"/>
-      <c r="L30" s="47"/>
-      <c r="M30" s="47"/>
-      <c r="N30" s="47"/>
-      <c r="O30" s="47"/>
-      <c r="P30" s="47"/>
-      <c r="Q30" s="47"/>
-      <c r="R30" s="59"/>
-      <c r="S30" s="47"/>
+      <c r="A30" s="27"/>
+      <c r="B30" s="37"/>
+      <c r="C30" s="27"/>
+      <c r="D30" s="27"/>
+      <c r="E30" s="27"/>
+      <c r="F30" s="27"/>
+      <c r="G30" s="27"/>
+      <c r="H30" s="27"/>
+      <c r="I30" s="27"/>
+      <c r="J30" s="27"/>
+      <c r="K30" s="27"/>
+      <c r="L30" s="27"/>
+      <c r="M30" s="27"/>
+      <c r="N30" s="27"/>
+      <c r="O30" s="27"/>
+      <c r="P30" s="27"/>
+      <c r="Q30" s="27"/>
+      <c r="R30" s="38"/>
+      <c r="S30" s="27"/>
     </row>
     <row r="31" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A31" s="47"/>
-      <c r="B31" s="58"/>
-      <c r="C31" s="47"/>
-      <c r="D31" s="47"/>
-      <c r="E31" s="47"/>
-      <c r="F31" s="47"/>
-      <c r="G31" s="47"/>
-      <c r="H31" s="47"/>
-      <c r="I31" s="47"/>
-      <c r="J31" s="47"/>
-      <c r="K31" s="47"/>
-      <c r="L31" s="47"/>
-      <c r="M31" s="47"/>
-      <c r="N31" s="47"/>
-      <c r="O31" s="47"/>
-      <c r="P31" s="47"/>
-      <c r="Q31" s="47"/>
-      <c r="R31" s="59"/>
-      <c r="S31" s="47"/>
+      <c r="A31" s="27"/>
+      <c r="B31" s="37"/>
+      <c r="C31" s="27"/>
+      <c r="D31" s="27"/>
+      <c r="E31" s="27"/>
+      <c r="F31" s="27"/>
+      <c r="G31" s="27"/>
+      <c r="H31" s="27"/>
+      <c r="I31" s="27"/>
+      <c r="J31" s="27"/>
+      <c r="K31" s="27"/>
+      <c r="L31" s="27"/>
+      <c r="M31" s="27"/>
+      <c r="N31" s="27"/>
+      <c r="O31" s="27"/>
+      <c r="P31" s="27"/>
+      <c r="Q31" s="27"/>
+      <c r="R31" s="38"/>
+      <c r="S31" s="27"/>
     </row>
     <row r="32" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A32" s="47"/>
-      <c r="B32" s="58"/>
-      <c r="C32" s="47"/>
-      <c r="D32" s="47"/>
-      <c r="E32" s="47"/>
-      <c r="F32" s="47"/>
-      <c r="G32" s="47"/>
-      <c r="H32" s="47"/>
-      <c r="I32" s="47"/>
-      <c r="J32" s="47"/>
-      <c r="K32" s="47"/>
-      <c r="L32" s="47"/>
-      <c r="M32" s="47"/>
-      <c r="N32" s="47"/>
-      <c r="O32" s="47"/>
-      <c r="P32" s="47"/>
-      <c r="Q32" s="47"/>
-      <c r="R32" s="59"/>
-      <c r="S32" s="47"/>
+      <c r="A32" s="27"/>
+      <c r="B32" s="37"/>
+      <c r="C32" s="27"/>
+      <c r="D32" s="27"/>
+      <c r="E32" s="27"/>
+      <c r="F32" s="27"/>
+      <c r="G32" s="27"/>
+      <c r="H32" s="27"/>
+      <c r="I32" s="27"/>
+      <c r="J32" s="27"/>
+      <c r="K32" s="27"/>
+      <c r="L32" s="27"/>
+      <c r="M32" s="27"/>
+      <c r="N32" s="27"/>
+      <c r="O32" s="27"/>
+      <c r="P32" s="27"/>
+      <c r="Q32" s="27"/>
+      <c r="R32" s="38"/>
+      <c r="S32" s="27"/>
     </row>
     <row r="33" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A33" s="47"/>
-      <c r="B33" s="58"/>
-      <c r="C33" s="47"/>
-      <c r="D33" s="47"/>
-      <c r="E33" s="47"/>
-      <c r="F33" s="47"/>
-      <c r="G33" s="47"/>
-      <c r="H33" s="47"/>
-      <c r="I33" s="47"/>
-      <c r="J33" s="47"/>
-      <c r="K33" s="47"/>
-      <c r="L33" s="47"/>
-      <c r="M33" s="47"/>
-      <c r="N33" s="47"/>
-      <c r="O33" s="47"/>
-      <c r="P33" s="47"/>
-      <c r="Q33" s="47"/>
-      <c r="R33" s="59"/>
-      <c r="S33" s="47"/>
+      <c r="A33" s="27"/>
+      <c r="B33" s="37"/>
+      <c r="C33" s="27"/>
+      <c r="D33" s="27"/>
+      <c r="E33" s="27"/>
+      <c r="F33" s="27"/>
+      <c r="G33" s="27"/>
+      <c r="H33" s="27"/>
+      <c r="I33" s="27"/>
+      <c r="J33" s="27"/>
+      <c r="K33" s="27"/>
+      <c r="L33" s="27"/>
+      <c r="M33" s="27"/>
+      <c r="N33" s="27"/>
+      <c r="O33" s="27"/>
+      <c r="P33" s="27"/>
+      <c r="Q33" s="27"/>
+      <c r="R33" s="38"/>
+      <c r="S33" s="27"/>
     </row>
     <row r="34" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A34" s="47"/>
-      <c r="B34" s="58"/>
-      <c r="C34" s="47"/>
-      <c r="D34" s="47"/>
-      <c r="E34" s="47"/>
-      <c r="F34" s="47"/>
-      <c r="G34" s="47"/>
-      <c r="H34" s="47"/>
-      <c r="I34" s="47"/>
-      <c r="J34" s="47"/>
-      <c r="K34" s="47"/>
-      <c r="L34" s="47"/>
-      <c r="M34" s="47"/>
-      <c r="N34" s="47"/>
-      <c r="O34" s="47"/>
-      <c r="P34" s="47"/>
-      <c r="Q34" s="47"/>
-      <c r="R34" s="59"/>
-      <c r="S34" s="47"/>
+      <c r="A34" s="27"/>
+      <c r="B34" s="37"/>
+      <c r="C34" s="27"/>
+      <c r="D34" s="27"/>
+      <c r="E34" s="27"/>
+      <c r="F34" s="27"/>
+      <c r="G34" s="27"/>
+      <c r="H34" s="27"/>
+      <c r="I34" s="27"/>
+      <c r="J34" s="27"/>
+      <c r="K34" s="27"/>
+      <c r="L34" s="27"/>
+      <c r="M34" s="27"/>
+      <c r="N34" s="27"/>
+      <c r="O34" s="27"/>
+      <c r="P34" s="27"/>
+      <c r="Q34" s="27"/>
+      <c r="R34" s="38"/>
+      <c r="S34" s="27"/>
     </row>
     <row r="35" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A35" s="47"/>
-      <c r="B35" s="58"/>
-      <c r="C35" s="47"/>
-      <c r="D35" s="47"/>
-      <c r="E35" s="47"/>
-      <c r="F35" s="47"/>
-      <c r="G35" s="47"/>
-      <c r="H35" s="47"/>
-      <c r="I35" s="47"/>
-      <c r="J35" s="47"/>
-      <c r="K35" s="47"/>
-      <c r="L35" s="47"/>
-      <c r="M35" s="47"/>
-      <c r="N35" s="47"/>
-      <c r="O35" s="47"/>
-      <c r="P35" s="47"/>
-      <c r="Q35" s="47"/>
-      <c r="R35" s="59"/>
-      <c r="S35" s="47"/>
+      <c r="A35" s="27"/>
+      <c r="B35" s="37"/>
+      <c r="C35" s="27"/>
+      <c r="D35" s="27"/>
+      <c r="E35" s="27"/>
+      <c r="F35" s="27"/>
+      <c r="G35" s="27"/>
+      <c r="H35" s="27"/>
+      <c r="I35" s="27"/>
+      <c r="J35" s="27"/>
+      <c r="K35" s="27"/>
+      <c r="L35" s="27"/>
+      <c r="M35" s="27"/>
+      <c r="N35" s="27"/>
+      <c r="O35" s="27"/>
+      <c r="P35" s="27"/>
+      <c r="Q35" s="27"/>
+      <c r="R35" s="38"/>
+      <c r="S35" s="27"/>
     </row>
     <row r="36" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A36" s="47"/>
-      <c r="B36" s="58"/>
-      <c r="C36" s="47"/>
-      <c r="D36" s="47"/>
-      <c r="E36" s="47"/>
-      <c r="F36" s="47"/>
-      <c r="G36" s="47"/>
-      <c r="H36" s="47"/>
-      <c r="I36" s="47"/>
-      <c r="J36" s="47"/>
-      <c r="K36" s="47"/>
-      <c r="L36" s="47"/>
-      <c r="M36" s="47"/>
-      <c r="N36" s="47"/>
-      <c r="O36" s="47"/>
-      <c r="P36" s="47"/>
-      <c r="Q36" s="47"/>
-      <c r="R36" s="59"/>
-      <c r="S36" s="47"/>
+      <c r="A36" s="27"/>
+      <c r="B36" s="37"/>
+      <c r="C36" s="27"/>
+      <c r="D36" s="27"/>
+      <c r="E36" s="27"/>
+      <c r="F36" s="27"/>
+      <c r="G36" s="27"/>
+      <c r="H36" s="27"/>
+      <c r="I36" s="27"/>
+      <c r="J36" s="27"/>
+      <c r="K36" s="27"/>
+      <c r="L36" s="27"/>
+      <c r="M36" s="27"/>
+      <c r="N36" s="27"/>
+      <c r="O36" s="27"/>
+      <c r="P36" s="27"/>
+      <c r="Q36" s="27"/>
+      <c r="R36" s="38"/>
+      <c r="S36" s="27"/>
     </row>
     <row r="37" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A37" s="47"/>
-      <c r="B37" s="60"/>
-      <c r="C37" s="61"/>
-      <c r="D37" s="61"/>
-      <c r="E37" s="61"/>
-      <c r="F37" s="61"/>
-      <c r="G37" s="61"/>
-      <c r="H37" s="61"/>
-      <c r="I37" s="61"/>
-      <c r="J37" s="61"/>
-      <c r="K37" s="61"/>
-      <c r="L37" s="61"/>
-      <c r="M37" s="61"/>
-      <c r="N37" s="61"/>
-      <c r="O37" s="61"/>
-      <c r="P37" s="61"/>
-      <c r="Q37" s="61"/>
-      <c r="R37" s="62"/>
-      <c r="S37" s="47"/>
+      <c r="A37" s="27"/>
+      <c r="B37" s="39"/>
+      <c r="C37" s="40"/>
+      <c r="D37" s="40"/>
+      <c r="E37" s="40"/>
+      <c r="F37" s="40"/>
+      <c r="G37" s="40"/>
+      <c r="H37" s="40"/>
+      <c r="I37" s="40"/>
+      <c r="J37" s="40"/>
+      <c r="K37" s="40"/>
+      <c r="L37" s="40"/>
+      <c r="M37" s="40"/>
+      <c r="N37" s="40"/>
+      <c r="O37" s="40"/>
+      <c r="P37" s="40"/>
+      <c r="Q37" s="40"/>
+      <c r="R37" s="41"/>
+      <c r="S37" s="27"/>
     </row>
     <row r="38" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A38" s="47"/>
-      <c r="B38" s="47"/>
-      <c r="C38" s="47"/>
-      <c r="D38" s="47"/>
-      <c r="E38" s="47"/>
-      <c r="F38" s="47"/>
-      <c r="G38" s="47"/>
-      <c r="H38" s="47"/>
-      <c r="I38" s="47"/>
-      <c r="J38" s="47"/>
-      <c r="K38" s="47"/>
-      <c r="L38" s="47"/>
-      <c r="M38" s="47"/>
-      <c r="N38" s="47"/>
-      <c r="O38" s="47"/>
-      <c r="P38" s="47"/>
-      <c r="Q38" s="47"/>
-      <c r="R38" s="47"/>
-      <c r="S38" s="47"/>
+      <c r="A38" s="27"/>
+      <c r="B38" s="27"/>
+      <c r="C38" s="27"/>
+      <c r="D38" s="27"/>
+      <c r="E38" s="27"/>
+      <c r="F38" s="27"/>
+      <c r="G38" s="27"/>
+      <c r="H38" s="27"/>
+      <c r="I38" s="27"/>
+      <c r="J38" s="27"/>
+      <c r="K38" s="27"/>
+      <c r="L38" s="27"/>
+      <c r="M38" s="27"/>
+      <c r="N38" s="27"/>
+      <c r="O38" s="27"/>
+      <c r="P38" s="27"/>
+      <c r="Q38" s="27"/>
+      <c r="R38" s="27"/>
+      <c r="S38" s="27"/>
     </row>
     <row r="39" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A39" s="47"/>
-      <c r="B39" s="47"/>
-      <c r="C39" s="47"/>
-      <c r="D39" s="47"/>
-      <c r="E39" s="47"/>
-      <c r="F39" s="47"/>
-      <c r="G39" s="47"/>
-      <c r="H39" s="47"/>
-      <c r="I39" s="47"/>
-      <c r="J39" s="47"/>
-      <c r="K39" s="47"/>
-      <c r="L39" s="47"/>
-      <c r="M39" s="47"/>
-      <c r="N39" s="47"/>
-      <c r="O39" s="47"/>
-      <c r="P39" s="47"/>
-      <c r="Q39" s="47"/>
-      <c r="R39" s="47"/>
-      <c r="S39" s="47"/>
+      <c r="A39" s="27"/>
+      <c r="B39" s="27"/>
+      <c r="C39" s="27"/>
+      <c r="D39" s="27"/>
+      <c r="E39" s="27"/>
+      <c r="F39" s="27"/>
+      <c r="G39" s="27"/>
+      <c r="H39" s="27"/>
+      <c r="I39" s="27"/>
+      <c r="J39" s="27"/>
+      <c r="K39" s="27"/>
+      <c r="L39" s="27"/>
+      <c r="M39" s="27"/>
+      <c r="N39" s="27"/>
+      <c r="O39" s="27"/>
+      <c r="P39" s="27"/>
+      <c r="Q39" s="27"/>
+      <c r="R39" s="27"/>
+      <c r="S39" s="27"/>
     </row>
     <row r="40" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A40" s="47"/>
-      <c r="B40" s="47"/>
-      <c r="C40" s="47"/>
-      <c r="D40" s="47"/>
-      <c r="E40" s="47"/>
-      <c r="F40" s="47"/>
-      <c r="G40" s="47"/>
-      <c r="H40" s="47"/>
-      <c r="I40" s="47"/>
-      <c r="J40" s="47"/>
-      <c r="K40" s="47"/>
-      <c r="L40" s="47"/>
-      <c r="M40" s="47"/>
-      <c r="N40" s="47"/>
-      <c r="O40" s="47"/>
-      <c r="P40" s="47"/>
-      <c r="Q40" s="47"/>
-      <c r="R40" s="47"/>
-      <c r="S40" s="47"/>
+      <c r="A40" s="27"/>
+      <c r="B40" s="27"/>
+      <c r="C40" s="27"/>
+      <c r="D40" s="27"/>
+      <c r="E40" s="27"/>
+      <c r="F40" s="27"/>
+      <c r="G40" s="27"/>
+      <c r="H40" s="27"/>
+      <c r="I40" s="27"/>
+      <c r="J40" s="27"/>
+      <c r="K40" s="27"/>
+      <c r="L40" s="27"/>
+      <c r="M40" s="27"/>
+      <c r="N40" s="27"/>
+      <c r="O40" s="27"/>
+      <c r="P40" s="27"/>
+      <c r="Q40" s="27"/>
+      <c r="R40" s="27"/>
+      <c r="S40" s="27"/>
     </row>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="B1:R2"/>
   </mergeCells>
-  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+  <printOptions horizontalCentered="1" verticalCentered="1"/>
+  <pageMargins left="0.51181102362204722" right="0.51181102362204722" top="0.78740157480314965" bottom="0.78740157480314965" header="0.31496062992125984" footer="0.31496062992125984"/>
   <pageSetup paperSize="9" scale="67" orientation="landscape" r:id="rId1"/>
   <drawing r:id="rId2"/>
 </worksheet>
@@ -4228,9 +4229,12 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0587B34E-A189-492A-AE93-696A64A8B090}">
+  <sheetPr>
+    <pageSetUpPr fitToPage="1"/>
+  </sheetPr>
   <dimension ref="B1:L58"/>
   <sheetViews>
-    <sheetView showGridLines="0" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
       <selection activeCell="D18" sqref="D18"/>
     </sheetView>
   </sheetViews>
@@ -4238,58 +4242,58 @@
   <cols>
     <col min="1" max="1" width="2.28515625" customWidth="1"/>
     <col min="2" max="2" width="14.85546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="18.42578125" style="32" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="18.42578125" style="17" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="16.7109375" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="15.7109375" customWidth="1"/>
     <col min="7" max="7" width="2.5703125" customWidth="1"/>
     <col min="8" max="8" width="14.85546875" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="18.42578125" style="32" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="18.42578125" style="17" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="16.7109375" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="15.7109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B1" s="17" t="s">
+      <c r="B1" s="58" t="s">
         <v>5</v>
       </c>
-      <c r="C1" s="18"/>
-      <c r="D1" s="18"/>
-      <c r="E1" s="18"/>
-      <c r="F1" s="18"/>
-      <c r="G1" s="18"/>
-      <c r="H1" s="18"/>
-      <c r="I1" s="18"/>
-      <c r="J1" s="18"/>
-      <c r="K1" s="18"/>
-      <c r="L1" s="19"/>
+      <c r="C1" s="59"/>
+      <c r="D1" s="59"/>
+      <c r="E1" s="59"/>
+      <c r="F1" s="59"/>
+      <c r="G1" s="59"/>
+      <c r="H1" s="59"/>
+      <c r="I1" s="59"/>
+      <c r="J1" s="59"/>
+      <c r="K1" s="59"/>
+      <c r="L1" s="60"/>
     </row>
     <row r="2" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B2" s="20"/>
-      <c r="C2" s="21"/>
-      <c r="D2" s="21"/>
-      <c r="E2" s="21"/>
-      <c r="F2" s="21"/>
-      <c r="G2" s="21"/>
-      <c r="H2" s="21"/>
-      <c r="I2" s="21"/>
-      <c r="J2" s="21"/>
-      <c r="K2" s="21"/>
-      <c r="L2" s="22"/>
+      <c r="B2" s="61"/>
+      <c r="C2" s="62"/>
+      <c r="D2" s="62"/>
+      <c r="E2" s="62"/>
+      <c r="F2" s="62"/>
+      <c r="G2" s="62"/>
+      <c r="H2" s="62"/>
+      <c r="I2" s="62"/>
+      <c r="J2" s="62"/>
+      <c r="K2" s="62"/>
+      <c r="L2" s="63"/>
     </row>
     <row r="3" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B3" s="26" t="s">
+      <c r="B3" s="64" t="s">
         <v>6</v>
       </c>
-      <c r="C3" s="27"/>
-      <c r="D3" s="28"/>
+      <c r="C3" s="65"/>
+      <c r="D3" s="66"/>
       <c r="E3" s="6"/>
       <c r="F3" s="6"/>
       <c r="G3" s="6"/>
       <c r="H3" s="52" t="s">
         <v>47</v>
       </c>
-      <c r="I3" s="37"/>
-      <c r="J3" s="38"/>
+      <c r="I3" s="53"/>
+      <c r="J3" s="54"/>
       <c r="K3" s="6"/>
       <c r="L3" s="7"/>
     </row>
@@ -4322,12 +4326,12 @@
       <c r="K4" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="L4" s="44" t="s">
+      <c r="L4" s="24" t="s">
         <v>32</v>
       </c>
     </row>
     <row r="5" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B5" s="54" t="s">
+      <c r="B5" s="33" t="s">
         <v>13</v>
       </c>
       <c r="C5" s="2" t="s">
@@ -4343,7 +4347,7 @@
         <v>4</v>
       </c>
       <c r="G5" s="6"/>
-      <c r="H5" s="36" t="s">
+      <c r="H5" s="21" t="s">
         <v>43</v>
       </c>
       <c r="I5" s="2" t="s">
@@ -4372,13 +4376,13 @@
       </c>
       <c r="F6" s="2"/>
       <c r="G6" s="6"/>
-      <c r="H6" s="64" t="s">
+      <c r="H6" s="43" t="s">
         <v>11</v>
       </c>
-      <c r="I6" s="34" t="s">
+      <c r="I6" s="19" t="s">
         <v>24</v>
       </c>
-      <c r="J6" s="34" t="s">
+      <c r="J6" s="19" t="s">
         <v>55</v>
       </c>
       <c r="K6" s="1" t="s">
@@ -4396,7 +4400,7 @@
       <c r="H7" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="I7" s="34" t="s">
+      <c r="I7" s="19" t="s">
         <v>25</v>
       </c>
       <c r="J7" s="1"/>
@@ -4406,18 +4410,18 @@
       <c r="L7" s="13"/>
     </row>
     <row r="8" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B8" s="29" t="s">
+      <c r="B8" s="67" t="s">
         <v>8</v>
       </c>
-      <c r="C8" s="30"/>
-      <c r="D8" s="31"/>
+      <c r="C8" s="68"/>
+      <c r="D8" s="69"/>
       <c r="E8" s="6"/>
       <c r="F8" s="6"/>
       <c r="G8" s="5"/>
       <c r="H8" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="I8" s="34" t="s">
+      <c r="I8" s="19" t="s">
         <v>1</v>
       </c>
       <c r="J8" s="1"/>
@@ -4443,10 +4447,10 @@
         <v>32</v>
       </c>
       <c r="G9" s="5"/>
-      <c r="H9" s="55" t="s">
+      <c r="H9" s="34" t="s">
         <v>13</v>
       </c>
-      <c r="I9" s="34" t="s">
+      <c r="I9" s="19" t="s">
         <v>1</v>
       </c>
       <c r="J9" s="1" t="s">
@@ -4458,7 +4462,7 @@
       <c r="L9" s="13"/>
     </row>
     <row r="10" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B10" s="56" t="s">
+      <c r="B10" s="35" t="s">
         <v>35</v>
       </c>
       <c r="C10" s="2" t="s">
@@ -4474,10 +4478,10 @@
         <v>4</v>
       </c>
       <c r="G10" s="5"/>
-      <c r="H10" s="56" t="s">
+      <c r="H10" s="35" t="s">
         <v>35</v>
       </c>
-      <c r="I10" s="34" t="s">
+      <c r="I10" s="19" t="s">
         <v>1</v>
       </c>
       <c r="J10" s="1" t="s">
@@ -4504,7 +4508,7 @@
       <c r="H11" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="I11" s="36" t="s">
+      <c r="I11" s="21" t="s">
         <v>1</v>
       </c>
       <c r="J11" s="1"/>
@@ -4523,7 +4527,7 @@
       <c r="H12" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="I12" s="34" t="s">
+      <c r="I12" s="19" t="s">
         <v>49</v>
       </c>
       <c r="J12" s="1"/>
@@ -4533,18 +4537,18 @@
       <c r="L12" s="13"/>
     </row>
     <row r="13" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B13" s="23" t="s">
+      <c r="B13" s="70" t="s">
         <v>23</v>
       </c>
-      <c r="C13" s="24"/>
-      <c r="D13" s="25"/>
+      <c r="C13" s="71"/>
+      <c r="D13" s="72"/>
       <c r="E13" s="6"/>
       <c r="F13" s="6"/>
       <c r="G13" s="6"/>
       <c r="H13" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="I13" s="34" t="s">
+      <c r="I13" s="19" t="s">
         <v>49</v>
       </c>
       <c r="J13" s="1"/>
@@ -4573,7 +4577,7 @@
       <c r="H14" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="I14" s="34" t="s">
+      <c r="I14" s="19" t="s">
         <v>49</v>
       </c>
       <c r="J14" s="1"/>
@@ -4600,7 +4604,7 @@
       <c r="H15" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="I15" s="34" t="s">
+      <c r="I15" s="19" t="s">
         <v>27</v>
       </c>
       <c r="J15" s="1"/>
@@ -4608,24 +4612,24 @@
       <c r="L15" s="13"/>
     </row>
     <row r="16" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B16" s="63" t="s">
+      <c r="B16" s="42" t="s">
         <v>11</v>
       </c>
-      <c r="C16" s="34" t="s">
+      <c r="C16" s="19" t="s">
         <v>24</v>
       </c>
-      <c r="D16" s="34" t="s">
+      <c r="D16" s="19" t="s">
         <v>55</v>
       </c>
-      <c r="E16" s="34" t="s">
+      <c r="E16" s="19" t="s">
         <v>4</v>
       </c>
-      <c r="F16" s="34"/>
+      <c r="F16" s="19"/>
       <c r="G16" s="6"/>
       <c r="H16" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="I16" s="34" t="s">
+      <c r="I16" s="19" t="s">
         <v>27</v>
       </c>
       <c r="J16" s="1"/>
@@ -4633,22 +4637,22 @@
       <c r="L16" s="13"/>
     </row>
     <row r="17" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B17" s="46" t="s">
+      <c r="B17" s="26" t="s">
         <v>12</v>
       </c>
-      <c r="C17" s="34" t="s">
+      <c r="C17" s="19" t="s">
         <v>25</v>
       </c>
-      <c r="D17" s="34"/>
-      <c r="E17" s="34" t="s">
+      <c r="D17" s="19"/>
+      <c r="E17" s="19" t="s">
         <v>4</v>
       </c>
-      <c r="F17" s="34"/>
+      <c r="F17" s="19"/>
       <c r="G17" s="6"/>
       <c r="H17" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="I17" s="34" t="s">
+      <c r="I17" s="19" t="s">
         <v>27</v>
       </c>
       <c r="J17" s="1"/>
@@ -4656,59 +4660,59 @@
       <c r="L17" s="13"/>
     </row>
     <row r="18" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B18" s="54" t="s">
+      <c r="B18" s="33" t="s">
         <v>13</v>
       </c>
-      <c r="C18" s="34" t="s">
+      <c r="C18" s="19" t="s">
         <v>1</v>
       </c>
-      <c r="D18" s="34" t="s">
+      <c r="D18" s="19" t="s">
         <v>33</v>
       </c>
-      <c r="E18" s="34" t="s">
+      <c r="E18" s="19" t="s">
         <v>4</v>
       </c>
-      <c r="F18" s="34"/>
+      <c r="F18" s="19"/>
       <c r="G18" s="6"/>
-      <c r="H18" s="47"/>
-      <c r="I18" s="48"/>
-      <c r="J18" s="47"/>
+      <c r="H18" s="27"/>
+      <c r="I18" s="28"/>
+      <c r="J18" s="27"/>
       <c r="K18" s="6"/>
       <c r="L18" s="7"/>
     </row>
     <row r="19" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B19" s="46" t="s">
+      <c r="B19" s="26" t="s">
         <v>14</v>
       </c>
-      <c r="C19" s="34" t="s">
+      <c r="C19" s="19" t="s">
         <v>1</v>
       </c>
-      <c r="D19" s="34"/>
-      <c r="E19" s="34" t="s">
+      <c r="D19" s="19"/>
+      <c r="E19" s="19" t="s">
         <v>4</v>
       </c>
-      <c r="F19" s="34"/>
-      <c r="G19" s="53"/>
-      <c r="H19" s="41" t="s">
+      <c r="F19" s="19"/>
+      <c r="G19" s="32"/>
+      <c r="H19" s="55" t="s">
         <v>46</v>
       </c>
-      <c r="I19" s="41"/>
-      <c r="J19" s="42"/>
+      <c r="I19" s="55"/>
+      <c r="J19" s="56"/>
       <c r="K19" s="6"/>
       <c r="L19" s="7"/>
     </row>
     <row r="20" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B20" s="46" t="s">
+      <c r="B20" s="26" t="s">
         <v>15</v>
       </c>
-      <c r="C20" s="34" t="s">
+      <c r="C20" s="19" t="s">
         <v>26</v>
       </c>
-      <c r="D20" s="34"/>
-      <c r="E20" s="34" t="s">
+      <c r="D20" s="19"/>
+      <c r="E20" s="19" t="s">
         <v>4</v>
       </c>
-      <c r="F20" s="34"/>
+      <c r="F20" s="19"/>
       <c r="G20" s="6"/>
       <c r="H20" s="3" t="s">
         <v>29</v>
@@ -4722,22 +4726,22 @@
       <c r="K20" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="L20" s="44" t="s">
+      <c r="L20" s="24" t="s">
         <v>32</v>
       </c>
     </row>
     <row r="21" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B21" s="46" t="s">
+      <c r="B21" s="26" t="s">
         <v>16</v>
       </c>
-      <c r="C21" s="33" t="s">
+      <c r="C21" s="18" t="s">
         <v>1</v>
       </c>
-      <c r="D21" s="33"/>
-      <c r="E21" s="33"/>
-      <c r="F21" s="33"/>
+      <c r="D21" s="18"/>
+      <c r="E21" s="18"/>
+      <c r="F21" s="18"/>
       <c r="G21" s="6"/>
-      <c r="H21" s="36" t="s">
+      <c r="H21" s="21" t="s">
         <v>48</v>
       </c>
       <c r="I21" s="2" t="s">
@@ -4754,23 +4758,23 @@
       </c>
     </row>
     <row r="22" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B22" s="45" t="s">
+      <c r="B22" s="25" t="s">
         <v>17</v>
       </c>
-      <c r="C22" s="35" t="s">
+      <c r="C22" s="20" t="s">
         <v>1</v>
       </c>
-      <c r="D22" s="35"/>
-      <c r="E22" s="35"/>
-      <c r="F22" s="35"/>
+      <c r="D22" s="20"/>
+      <c r="E22" s="20"/>
+      <c r="F22" s="20"/>
       <c r="G22" s="6"/>
-      <c r="H22" s="64" t="s">
+      <c r="H22" s="43" t="s">
         <v>11</v>
       </c>
-      <c r="I22" s="34" t="s">
+      <c r="I22" s="19" t="s">
         <v>24</v>
       </c>
-      <c r="J22" s="34" t="s">
+      <c r="J22" s="19" t="s">
         <v>55</v>
       </c>
       <c r="K22" s="1" t="s">
@@ -4779,20 +4783,20 @@
       <c r="L22" s="13"/>
     </row>
     <row r="23" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B23" s="49" t="s">
+      <c r="B23" s="29" t="s">
         <v>18</v>
       </c>
-      <c r="C23" s="35" t="s">
+      <c r="C23" s="20" t="s">
         <v>27</v>
       </c>
-      <c r="D23" s="35"/>
-      <c r="E23" s="35"/>
-      <c r="F23" s="35"/>
+      <c r="D23" s="20"/>
+      <c r="E23" s="20"/>
+      <c r="F23" s="20"/>
       <c r="G23" s="6"/>
-      <c r="H23" s="34" t="s">
+      <c r="H23" s="19" t="s">
         <v>12</v>
       </c>
-      <c r="I23" s="34" t="s">
+      <c r="I23" s="19" t="s">
         <v>25</v>
       </c>
       <c r="J23" s="1"/>
@@ -4802,20 +4806,20 @@
       <c r="L23" s="13"/>
     </row>
     <row r="24" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B24" s="49" t="s">
+      <c r="B24" s="29" t="s">
         <v>19</v>
       </c>
-      <c r="C24" s="35" t="s">
+      <c r="C24" s="20" t="s">
         <v>27</v>
       </c>
-      <c r="D24" s="35"/>
-      <c r="E24" s="35"/>
-      <c r="F24" s="35"/>
+      <c r="D24" s="20"/>
+      <c r="E24" s="20"/>
+      <c r="F24" s="20"/>
       <c r="G24" s="6"/>
-      <c r="H24" s="55" t="s">
+      <c r="H24" s="34" t="s">
         <v>13</v>
       </c>
-      <c r="I24" s="34" t="s">
+      <c r="I24" s="19" t="s">
         <v>1</v>
       </c>
       <c r="J24" s="1" t="s">
@@ -4827,20 +4831,20 @@
       <c r="L24" s="13"/>
     </row>
     <row r="25" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B25" s="49" t="s">
+      <c r="B25" s="29" t="s">
         <v>20</v>
       </c>
-      <c r="C25" s="34" t="s">
+      <c r="C25" s="19" t="s">
         <v>27</v>
       </c>
-      <c r="D25" s="34"/>
-      <c r="E25" s="34"/>
-      <c r="F25" s="34"/>
+      <c r="D25" s="19"/>
+      <c r="E25" s="19"/>
+      <c r="F25" s="19"/>
       <c r="G25" s="6"/>
-      <c r="H25" s="34" t="s">
+      <c r="H25" s="19" t="s">
         <v>14</v>
       </c>
-      <c r="I25" s="34" t="s">
+      <c r="I25" s="19" t="s">
         <v>1</v>
       </c>
       <c r="J25" s="1"/>
@@ -4850,83 +4854,83 @@
       <c r="L25" s="13"/>
     </row>
     <row r="26" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B26" s="46" t="s">
+      <c r="B26" s="26" t="s">
         <v>21</v>
       </c>
-      <c r="C26" s="34" t="s">
+      <c r="C26" s="19" t="s">
         <v>28</v>
       </c>
-      <c r="D26" s="34"/>
-      <c r="E26" s="34"/>
-      <c r="F26" s="34"/>
+      <c r="D26" s="19"/>
+      <c r="E26" s="19"/>
+      <c r="F26" s="19"/>
       <c r="G26" s="6"/>
-      <c r="H26" s="34" t="s">
+      <c r="H26" s="19" t="s">
         <v>44</v>
       </c>
-      <c r="I26" s="34" t="s">
+      <c r="I26" s="19" t="s">
         <v>49</v>
       </c>
-      <c r="J26" s="34"/>
+      <c r="J26" s="19"/>
       <c r="K26" s="1" t="s">
         <v>4</v>
       </c>
       <c r="L26" s="13"/>
     </row>
     <row r="27" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B27" s="46" t="s">
+      <c r="B27" s="26" t="s">
         <v>22</v>
       </c>
-      <c r="C27" s="35" t="s">
+      <c r="C27" s="20" t="s">
         <v>25</v>
       </c>
       <c r="D27" s="1"/>
       <c r="E27" s="1"/>
       <c r="F27" s="1"/>
       <c r="G27" s="6"/>
-      <c r="H27" s="34" t="s">
+      <c r="H27" s="19" t="s">
         <v>15</v>
       </c>
-      <c r="I27" s="34" t="s">
+      <c r="I27" s="19" t="s">
         <v>49</v>
       </c>
-      <c r="J27" s="34"/>
+      <c r="J27" s="19"/>
       <c r="K27" s="1" t="s">
         <v>4</v>
       </c>
       <c r="L27" s="13"/>
     </row>
     <row r="28" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B28" s="50"/>
+      <c r="B28" s="30"/>
       <c r="C28" s="4"/>
       <c r="D28" s="6"/>
       <c r="E28" s="6"/>
       <c r="F28" s="6"/>
       <c r="G28" s="6"/>
-      <c r="H28" s="34" t="s">
+      <c r="H28" s="19" t="s">
         <v>45</v>
       </c>
-      <c r="I28" s="34" t="s">
+      <c r="I28" s="19" t="s">
         <v>27</v>
       </c>
-      <c r="J28" s="34"/>
+      <c r="J28" s="19"/>
       <c r="K28" s="1" t="s">
         <v>4</v>
       </c>
       <c r="L28" s="13"/>
     </row>
     <row r="29" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B29" s="65" t="s">
+      <c r="B29" s="50" t="s">
         <v>50</v>
       </c>
-      <c r="C29" s="66"/>
-      <c r="D29" s="66"/>
+      <c r="C29" s="51"/>
+      <c r="D29" s="51"/>
       <c r="E29" s="6"/>
       <c r="F29" s="6"/>
       <c r="G29" s="6"/>
-      <c r="H29" s="56" t="s">
+      <c r="H29" s="35" t="s">
         <v>35</v>
       </c>
-      <c r="I29" s="34" t="s">
+      <c r="I29" s="19" t="s">
         <v>1</v>
       </c>
       <c r="J29" s="1" t="s">
@@ -4961,10 +4965,10 @@
       <c r="L30" s="7"/>
     </row>
     <row r="31" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B31" s="63" t="s">
+      <c r="B31" s="42" t="s">
         <v>11</v>
       </c>
-      <c r="C31" s="34" t="s">
+      <c r="C31" s="19" t="s">
         <v>24</v>
       </c>
       <c r="D31" s="2" t="s">
@@ -4977,11 +4981,11 @@
         <v>4</v>
       </c>
       <c r="G31" s="6"/>
-      <c r="H31" s="43" t="s">
+      <c r="H31" s="57" t="s">
         <v>58</v>
       </c>
-      <c r="I31" s="43"/>
-      <c r="J31" s="43"/>
+      <c r="I31" s="57"/>
+      <c r="J31" s="57"/>
       <c r="K31" s="6"/>
       <c r="L31" s="7"/>
     </row>
@@ -5010,7 +5014,7 @@
       <c r="K32" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="L32" s="44" t="s">
+      <c r="L32" s="24" t="s">
         <v>32</v>
       </c>
     </row>
@@ -5027,13 +5031,13 @@
       </c>
       <c r="F33" s="1"/>
       <c r="G33" s="6"/>
-      <c r="H33" s="64" t="s">
+      <c r="H33" s="43" t="s">
         <v>11</v>
       </c>
-      <c r="I33" s="34" t="s">
+      <c r="I33" s="19" t="s">
         <v>24</v>
       </c>
-      <c r="J33" s="34" t="s">
+      <c r="J33" s="19" t="s">
         <v>55</v>
       </c>
       <c r="K33" s="2" t="s">
@@ -5096,7 +5100,7 @@
     <row r="36" spans="2:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B36" s="14"/>
       <c r="C36" s="15"/>
-      <c r="D36" s="51"/>
+      <c r="D36" s="31"/>
       <c r="E36" s="15"/>
       <c r="F36" s="15"/>
       <c r="G36" s="15"/>
@@ -5108,111 +5112,111 @@
     </row>
     <row r="37" spans="2:12" x14ac:dyDescent="0.25">
       <c r="C37"/>
-      <c r="D37" s="32"/>
+      <c r="D37" s="17"/>
       <c r="I37"/>
     </row>
     <row r="38" spans="2:12" x14ac:dyDescent="0.25">
       <c r="C38"/>
-      <c r="D38" s="32"/>
+      <c r="D38" s="17"/>
       <c r="I38"/>
     </row>
     <row r="39" spans="2:12" x14ac:dyDescent="0.25">
       <c r="C39"/>
-      <c r="D39" s="32"/>
+      <c r="D39" s="17"/>
       <c r="I39"/>
     </row>
     <row r="40" spans="2:12" x14ac:dyDescent="0.25">
       <c r="C40"/>
-      <c r="D40" s="32"/>
+      <c r="D40" s="17"/>
       <c r="I40"/>
     </row>
     <row r="41" spans="2:12" x14ac:dyDescent="0.25">
       <c r="C41"/>
-      <c r="D41" s="32"/>
+      <c r="D41" s="17"/>
       <c r="I41"/>
     </row>
     <row r="42" spans="2:12" x14ac:dyDescent="0.25">
       <c r="C42"/>
-      <c r="D42" s="32"/>
+      <c r="D42" s="17"/>
       <c r="I42"/>
     </row>
     <row r="43" spans="2:12" x14ac:dyDescent="0.25">
       <c r="C43"/>
-      <c r="D43" s="32"/>
+      <c r="D43" s="17"/>
       <c r="I43"/>
     </row>
     <row r="44" spans="2:12" x14ac:dyDescent="0.25">
       <c r="C44"/>
-      <c r="D44" s="32"/>
+      <c r="D44" s="17"/>
       <c r="I44"/>
     </row>
     <row r="45" spans="2:12" x14ac:dyDescent="0.25">
       <c r="C45"/>
-      <c r="D45" s="32"/>
+      <c r="D45" s="17"/>
       <c r="I45"/>
     </row>
     <row r="46" spans="2:12" x14ac:dyDescent="0.25">
       <c r="C46"/>
-      <c r="D46" s="32"/>
+      <c r="D46" s="17"/>
       <c r="I46"/>
     </row>
     <row r="47" spans="2:12" x14ac:dyDescent="0.25">
       <c r="C47"/>
-      <c r="D47" s="32"/>
+      <c r="D47" s="17"/>
       <c r="I47"/>
     </row>
     <row r="48" spans="2:12" x14ac:dyDescent="0.25">
       <c r="C48"/>
-      <c r="D48" s="32"/>
+      <c r="D48" s="17"/>
       <c r="I48"/>
     </row>
     <row r="49" spans="2:9" x14ac:dyDescent="0.25">
       <c r="C49"/>
-      <c r="D49" s="32"/>
+      <c r="D49" s="17"/>
       <c r="I49"/>
     </row>
     <row r="50" spans="2:9" x14ac:dyDescent="0.25">
       <c r="C50"/>
-      <c r="D50" s="32"/>
+      <c r="D50" s="17"/>
       <c r="I50"/>
     </row>
     <row r="51" spans="2:9" x14ac:dyDescent="0.25">
       <c r="C51"/>
-      <c r="D51" s="32"/>
+      <c r="D51" s="17"/>
       <c r="I51"/>
     </row>
     <row r="52" spans="2:9" x14ac:dyDescent="0.25">
       <c r="C52"/>
-      <c r="D52" s="32"/>
+      <c r="D52" s="17"/>
       <c r="I52"/>
     </row>
     <row r="53" spans="2:9" x14ac:dyDescent="0.25">
       <c r="C53"/>
-      <c r="D53" s="32"/>
+      <c r="D53" s="17"/>
       <c r="I53"/>
     </row>
     <row r="54" spans="2:9" x14ac:dyDescent="0.25">
       <c r="C54"/>
-      <c r="D54" s="32"/>
+      <c r="D54" s="17"/>
     </row>
     <row r="55" spans="2:9" x14ac:dyDescent="0.25">
       <c r="C55"/>
-      <c r="D55" s="32"/>
+      <c r="D55" s="17"/>
     </row>
     <row r="56" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B56" s="39"/>
-      <c r="C56" s="40"/>
-      <c r="D56" s="39"/>
+      <c r="B56" s="22"/>
+      <c r="C56" s="23"/>
+      <c r="D56" s="22"/>
     </row>
     <row r="57" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B57" s="39"/>
-      <c r="C57" s="40"/>
-      <c r="D57" s="39"/>
+      <c r="B57" s="22"/>
+      <c r="C57" s="23"/>
+      <c r="D57" s="22"/>
     </row>
     <row r="58" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B58" s="39"/>
-      <c r="C58" s="40"/>
-      <c r="D58" s="39"/>
+      <c r="B58" s="22"/>
+      <c r="C58" s="23"/>
+      <c r="D58" s="22"/>
     </row>
   </sheetData>
   <mergeCells count="8">
@@ -5225,7 +5229,8 @@
     <mergeCell ref="B8:D8"/>
     <mergeCell ref="B13:D13"/>
   </mergeCells>
-  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <printOptions horizontalCentered="1" verticalCentered="1"/>
+  <pageMargins left="0.19685039370078741" right="0.19685039370078741" top="0.19685039370078741" bottom="0.19685039370078741" header="0.31496062992125984" footer="0.31496062992125984"/>
+  <pageSetup paperSize="9" scale="93" orientation="landscape" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>